<commit_message>
LangRef div and various formatting
</commit_message>
<xml_diff>
--- a/src/documentation/MessagesInLangRef.xlsx
+++ b/src/documentation/MessagesInLangRef.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>id="TypeCompileError"</t>
   </si>
@@ -343,9 +343,6 @@
     <t>id="paramNameNotSameAsItsMethod"</t>
   </si>
   <si>
-    <t xml:space="preserve"> Parameter ... may not have the same name as the method in which it is defined.</t>
-  </si>
-  <si>
     <t>id="ArgListField"</t>
   </si>
   <si>
@@ -464,6 +461,21 @@
   </si>
   <si>
     <t>ReferenceError: Cannot access '[name]' before initialization</t>
+  </si>
+  <si>
+    <t>id="divDeprecated"</t>
+  </si>
+  <si>
+    <t>div' is deprecated. Recommended code for interger divistion is e.g. (10/3).floor()</t>
+  </si>
+  <si>
+    <t>Parameter ... may not have the same name as the method in which it is defined.</t>
+  </si>
+  <si>
+    <t>id="methodDeprecated"</t>
+  </si>
+  <si>
+    <t>Code change suggested. Method was deprecated in v1.7.</t>
   </si>
 </sst>
 </file>
@@ -500,9 +512,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -1322,167 +1335,183 @@
         <v>108</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>